<commit_message>
Nouvelles fonction + organisation code
</commit_message>
<xml_diff>
--- a/Plan de test.xlsx
+++ b/Plan de test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJET FORMATION\Formation Projet 5\BenjaminBonnefoy_P5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC178D83-1CA4-4D31-BB2E-04C0E5EA5AB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57374F85-85C0-45DC-BA5E-7A7B92E297C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3435" yWindow="1215" windowWidth="21195" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -87,6 +87,69 @@
   <si>
     <t>Cette fonction étant appélé dans la fonction précédente, elle possède le même problème. Si la première fonction ne renvoi rien alors celle la non plus.</t>
   </si>
+  <si>
+    <t>deleteItem</t>
+  </si>
+  <si>
+    <t>La fonction pourrait ne pas réussir à supprimer les éléments ou à ne pas réussir à recharger l'HTML correctement.</t>
+  </si>
+  <si>
+    <t>clearStorage</t>
+  </si>
+  <si>
+    <t>La fonction pourrait ne pas réussir à supprimer le contenu du localStorage ou à ne pas réussir à recharger l'HTML correctement.</t>
+  </si>
+  <si>
+    <t>panier.js</t>
+  </si>
+  <si>
+    <t>resetHtml</t>
+  </si>
+  <si>
+    <t>La fonction doit supprimer l'intégralité du localStorage grâce à la méthode .clear() et recharger l'HTML de la page à l'aide de la fonction resetHtml.</t>
+  </si>
+  <si>
+    <t>La fonction doit supprimer l'élément cibler du panier au click du button associé et recharger l'HTML de la page à l'aide de la fonction resetHtml.</t>
+  </si>
+  <si>
+    <t>La fonction affiche tout le tableau panier des produits enregistré dans le localStorage.</t>
+  </si>
+  <si>
+    <t>Appeler la fonction avec 2 paramètre, boxPanier correspondant au bloc contenant le panier et le JSON.parse du localStorage. Si la console ne renvoie aucune erreur alors tout c'est charger correctement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cette fonction appelant plusieurs autres fonctions, elle pourrait renvoyé des erreurs dans la console lié aux erreurs présentes dans les autres fonctions. </t>
+  </si>
+  <si>
+    <t>Appeler la fonction avec 3 paramètre, le JSON.parse du localStorage, le i de la boucle sur les éléments présent dans le localStorage et boxPanier correspondant au bloc contenant le panier. Lors du click sur le bouton supprimer, l'élément devrait se retirer.</t>
+  </si>
+  <si>
+    <t>Appeler la fonction avec 2 paramètre, le JSON.parse du localStorage et boxPanier correspondant au bloc contenant le panier. Lors du click sur le bouton "vider le panier", le panier devrait afficher "le panier est vide".</t>
+  </si>
+  <si>
+    <t>saveOrder</t>
+  </si>
+  <si>
+    <t>La fonction doit sauvegarder dans le localStorage les informations relatif à la commande (Prix, Nom/prénom, ID) et renvoyer sur la page de confirmation de commande.</t>
+  </si>
+  <si>
+    <t>Appeler la fonction avec comme paramètre la response.json() de la requête post. Lors du click sur le bouton "envoyer" la page de  confirmation de commande doit s'ouvrir avec les bonnes informations.</t>
+  </si>
+  <si>
+    <t>La fonction pourrait ne pas enregistrer les bonnes informations de la commande ou ne pas réussir à renvoyer sur la page de confirmation de commande.</t>
+  </si>
+  <si>
+    <t>71 à 80</t>
+  </si>
+  <si>
+    <t>84 à 90</t>
+  </si>
+  <si>
+    <t>94 à 106</t>
+  </si>
+  <si>
+    <t>9 à 106</t>
+  </si>
 </sst>
 </file>
 
@@ -139,22 +202,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -377,28 +443,28 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="50.5703125" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" customWidth="1"/>
-    <col min="6" max="6" width="42.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="50.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="42.7109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -410,136 +476,196 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-    </row>
-    <row r="2" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="3" spans="1:26" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="4" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+    <row r="5" spans="1:26" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D15" s="4"/>

</xml_diff>

<commit_message>
Maj plan de test
</commit_message>
<xml_diff>
--- a/Plan de test.xlsx
+++ b/Plan de test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJET FORMATION\Formation Projet 5\BenjaminBonnefoy_P5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57374F85-85C0-45DC-BA5E-7A7B92E297C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1B78CE-6B68-4A97-95E8-57B5BA2AE093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -149,6 +149,21 @@
   </si>
   <si>
     <t>9 à 106</t>
+  </si>
+  <si>
+    <t>110 à 131</t>
+  </si>
+  <si>
+    <t>popupAdd</t>
+  </si>
+  <si>
+    <t>La fonction doit afficher un pop-up de confimation d'ajout dans le panier de l'élément sélectionné comprenant sa quantité et sa couleur.</t>
+  </si>
+  <si>
+    <t>Appeler la fonction avec comme paramètre le nouveau Produit créé de la classe Produit et mainProduit correspondant au bloc comprenant les détails du produit. Lors du click "Ajouter au panier" le pop-up devrait s'afficher avec les bonnes informations.</t>
+  </si>
+  <si>
+    <t>La fonction pourrait ne pas envoyer les bonnes informations ou ne pas afficher correctement le pop-up si l'élément ne s'est pas créé correctement.</t>
   </si>
 </sst>
 </file>
@@ -440,11 +455,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -617,30 +632,45 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B9" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D10" s="3"/>
@@ -667,10 +697,10 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+    <row r="15" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D16" s="4"/>
@@ -692,7 +722,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -817,7 +847,7 @@
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
@@ -5587,6 +5617,11 @@
       <c r="E998" s="4"/>
       <c r="F998" s="4"/>
     </row>
+    <row r="999" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D999" s="4"/>
+      <c r="E999" s="4"/>
+      <c r="F999" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modification switch et suppression d'espace
</commit_message>
<xml_diff>
--- a/Plan de test.xlsx
+++ b/Plan de test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJET FORMATION\Formation Projet 5\BenjaminBonnefoy_P5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1B78CE-6B68-4A97-95E8-57B5BA2AE093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14C7EC2-5F2A-4853-8A70-957F45940EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,12 +44,6 @@
   </si>
   <si>
     <t>8 à 18</t>
-  </si>
-  <si>
-    <t>22 à 55</t>
-  </si>
-  <si>
-    <t>59 à 67</t>
   </si>
   <si>
     <t>createHTML</t>
@@ -139,21 +133,6 @@
     <t>La fonction pourrait ne pas enregistrer les bonnes informations de la commande ou ne pas réussir à renvoyer sur la page de confirmation de commande.</t>
   </si>
   <si>
-    <t>71 à 80</t>
-  </si>
-  <si>
-    <t>84 à 90</t>
-  </si>
-  <si>
-    <t>94 à 106</t>
-  </si>
-  <si>
-    <t>9 à 106</t>
-  </si>
-  <si>
-    <t>110 à 131</t>
-  </si>
-  <si>
     <t>popupAdd</t>
   </si>
   <si>
@@ -164,6 +143,27 @@
   </si>
   <si>
     <t>La fonction pourrait ne pas envoyer les bonnes informations ou ne pas afficher correctement le pop-up si l'élément ne s'est pas créé correctement.</t>
+  </si>
+  <si>
+    <t>22 à 46</t>
+  </si>
+  <si>
+    <t>50 à 58</t>
+  </si>
+  <si>
+    <t>62 à 71</t>
+  </si>
+  <si>
+    <t>75 à 81</t>
+  </si>
+  <si>
+    <t>85 à 97</t>
+  </si>
+  <si>
+    <t>101 à 122</t>
+  </si>
+  <si>
+    <t>9 à 100</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -520,16 +520,16 @@
         <v>7</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -537,19 +537,19 @@
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -557,19 +557,19 @@
         <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -577,19 +577,19 @@
         <v>6</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -597,19 +597,19 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -617,19 +617,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -637,39 +637,39 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="C9" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>